<commit_message>
implemented the next step rejected
</commit_message>
<xml_diff>
--- a/docs/IDs_from_MAKE_Camunda.xlsx
+++ b/docs/IDs_from_MAKE_Camunda.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master\05_Semester\Digitalization of Business Processes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike Vontobel\DigiBP_Team_Blueberries\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF267AE1-59D2-459C-BEFC-14EA14351E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D45798-EBD9-418B-9F6D-F068503EE90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>ID-Number</t>
-  </si>
-  <si>
     <t>New request for a leave</t>
   </si>
   <si>
@@ -138,22 +135,37 @@
     <t>Gateway</t>
   </si>
   <si>
-    <t>${absence_from_type_decision=="rejected"}</t>
-  </si>
-  <si>
     <t>Rejected</t>
   </si>
   <si>
     <t>Need more information</t>
   </si>
   <si>
-    <t>${absence_from_type_decision=="prov-approved"}</t>
-  </si>
-  <si>
-    <t>${absence_from_type_decision=="approved"}</t>
-  </si>
-  <si>
     <t>Automatically approuved</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>${Output_absenceFromType=="rejected"}</t>
+  </si>
+  <si>
+    <t>${Output_absenceFromType=="prov-approved"}</t>
+  </si>
+  <si>
+    <t>${Output_absenceFromType=="auto-approved"}</t>
+  </si>
+  <si>
+    <t>Service Task</t>
+  </si>
+  <si>
+    <t>Inform the employee</t>
+  </si>
+  <si>
+    <t>ID-Number / Topic</t>
+  </si>
+  <si>
+    <t>informEmployee</t>
   </si>
 </sst>
 </file>
@@ -229,12 +241,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{126E6340-5723-4B4A-A7DF-102EE820FAA5}" name="Table1" displayName="Table1" ref="B2:E34" totalsRowShown="0">
-  <autoFilter ref="B2:E34" xr:uid="{126E6340-5723-4B4A-A7DF-102EE820FAA5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{126E6340-5723-4B4A-A7DF-102EE820FAA5}" name="Table1" displayName="Table1" ref="B2:E35" totalsRowShown="0">
+  <autoFilter ref="B2:E35" xr:uid="{126E6340-5723-4B4A-A7DF-102EE820FAA5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{11157681-B50A-47E1-8358-3F99B05BD726}" name="What it is?"/>
     <tableColumn id="3" xr3:uid="{AA3DE658-58E5-42C0-974C-6EE6E9B4DF32}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{30CB5B4D-0EC7-4E25-8525-FF0DAB8811E9}" name="ID-Number"/>
+    <tableColumn id="2" xr3:uid="{30CB5B4D-0EC7-4E25-8525-FF0DAB8811E9}" name="ID-Number / Topic"/>
     <tableColumn id="4" xr3:uid="{12BEBCAB-3451-429A-A6EA-784E8A28EBBB}" name="Variables"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -504,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E23"/>
+  <dimension ref="B2:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,165 +533,162 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E18" t="s">
         <v>31</v>
-      </c>
-      <c r="E17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="C22" t="s">
         <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>39</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
@@ -687,10 +696,29 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>